<commit_message>
Manejo de errores e interfaz de usuario
</commit_message>
<xml_diff>
--- a/Casos de prueba Reto Codigo limpio.xlsx
+++ b/Casos de prueba Reto Codigo limpio.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Santiago\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Santiago\Desktop\Codigo Limpio\Codigo limpio 2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{164308DE-EED3-4E72-AD51-EACEFE2DC97D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{90B4E4BE-DC0E-45DC-8057-F934B18D4764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{38C97209-6CC1-444D-9DD9-194BB269E202}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>Casos normales</t>
   </si>
@@ -147,6 +147,18 @@
   </si>
   <si>
     <t>#ERROR EL VALOR DEL IVA NO PUEDE SER MENOR A 0</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>Valor invalido de impuesto a bolsa</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>#ERROR DEBE TENR UN VALOR DE STRING VALIDO</t>
   </si>
 </sst>
 </file>
@@ -214,15 +226,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -234,13 +237,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -577,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B421A44E-3DE2-44E4-A124-F71E8BDBE745}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,465 +611,465 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="4" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="2"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="3">
         <v>65000</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="4">
         <v>0.19</v>
       </c>
-      <c r="D4" s="7">
-        <v>0</v>
-      </c>
-      <c r="E4" s="7">
-        <v>0</v>
-      </c>
-      <c r="F4" s="8" t="s">
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="3">
         <f>B4*D4</f>
         <v>0</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="3">
         <f>B4*E4</f>
         <v>0</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="3">
         <f>IF(F4="True",70,0)</f>
         <v>70</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="3">
         <f>B4*C4</f>
         <v>12350</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="3">
         <f>G4+H4+I4+J4+B4</f>
         <v>77420</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="1">
         <v>150000</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="6">
         <v>0.05</v>
       </c>
-      <c r="D5" s="10">
-        <v>0</v>
-      </c>
-      <c r="E5" s="10">
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6">
         <v>0.05</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="3">
         <f t="shared" ref="G5:G13" si="0">B5*D5</f>
         <v>0</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="3">
         <f t="shared" ref="H5:H13" si="1">B5*E5</f>
         <v>7500</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="3">
         <f t="shared" ref="I5:I13" si="2">IF(F5="True",70,0)</f>
         <v>70</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="3">
         <f t="shared" ref="J5:J13" si="3">B5*C5</f>
         <v>7500</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="3">
         <f t="shared" ref="K5:K13" si="4">G5+H5+I5+J5+B5</f>
         <v>165070</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="1">
         <v>230000</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="6">
         <v>0.19</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="6">
         <v>0.08</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="6">
         <v>0.05</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="3">
         <f t="shared" si="0"/>
         <v>18400</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="3">
         <f t="shared" si="1"/>
         <v>11500</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="3">
         <f t="shared" si="3"/>
         <v>43700</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="3">
         <f t="shared" si="4"/>
         <v>303600</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="1">
         <v>315000</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="6">
         <v>0.19</v>
       </c>
-      <c r="D7" s="10">
-        <v>0</v>
-      </c>
-      <c r="E7" s="11">
-        <v>0</v>
-      </c>
-      <c r="F7" s="8" t="s">
+      <c r="D7" s="6">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="3">
         <f t="shared" si="2"/>
         <v>70</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="3">
         <f t="shared" si="3"/>
         <v>59850</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="3">
         <f t="shared" si="4"/>
         <v>374920</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="1">
         <v>410000</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="6">
         <v>0.19</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="6">
         <v>0.16</v>
       </c>
-      <c r="E8" s="10">
-        <v>0</v>
-      </c>
-      <c r="F8" s="8" t="s">
+      <c r="E8" s="6">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>65600</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="3">
         <f t="shared" si="2"/>
         <v>70</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="3">
         <f t="shared" si="3"/>
         <v>77900</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="3">
         <f t="shared" si="4"/>
         <v>553570</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="1">
         <v>52500</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="6">
         <v>0.05</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="6">
         <v>0.04</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="6">
         <v>0.05</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>2100</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="3">
         <f t="shared" si="1"/>
         <v>2625</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="3">
         <f t="shared" si="3"/>
         <v>2625</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="3">
         <f t="shared" si="4"/>
         <v>59850</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="1">
         <v>600000</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="6">
         <v>0.19</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="6">
         <v>0.04</v>
       </c>
-      <c r="E10" s="10">
-        <v>0</v>
-      </c>
-      <c r="F10" s="8" t="s">
+      <c r="E10" s="6">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>24000</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="3">
         <f t="shared" si="2"/>
         <v>70</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J10" s="3">
         <f t="shared" si="3"/>
         <v>114000</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="3">
         <f t="shared" si="4"/>
         <v>738070</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="1">
         <v>7200</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="6">
         <v>0.05</v>
       </c>
-      <c r="D11" s="10">
-        <v>0</v>
-      </c>
-      <c r="E11" s="10">
+      <c r="D11" s="6">
+        <v>0</v>
+      </c>
+      <c r="E11" s="6">
         <v>0</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J11" s="6">
+      <c r="J11" s="3">
         <f t="shared" si="3"/>
         <v>360</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K11" s="3">
         <f t="shared" si="4"/>
         <v>7560</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="1">
         <v>850000</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="6">
         <v>0.19</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="6">
         <v>0.16</v>
       </c>
-      <c r="E12" s="10">
-        <v>0</v>
-      </c>
-      <c r="F12" s="8" t="s">
+      <c r="E12" s="6">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="3">
         <f t="shared" si="0"/>
         <v>136000</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="3">
         <f t="shared" si="2"/>
         <v>70</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J12" s="3">
         <f t="shared" si="3"/>
         <v>161500</v>
       </c>
-      <c r="K12" s="6">
+      <c r="K12" s="3">
         <f t="shared" si="4"/>
         <v>1147570</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="1">
         <v>93000</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="6">
         <v>0.19</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="6">
         <v>0.08</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="6">
         <v>0.05</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="3">
         <f t="shared" si="0"/>
         <v>7440</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="3">
         <f t="shared" si="1"/>
         <v>4650</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J13" s="6">
+      <c r="J13" s="3">
         <f t="shared" si="3"/>
         <v>17670</v>
       </c>
-      <c r="K13" s="6">
+      <c r="K13" s="3">
         <f t="shared" si="4"/>
         <v>122760</v>
       </c>
@@ -1076,7 +1088,7 @@
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="1"/>
@@ -1094,38 +1106,38 @@
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="3">
         <v>35000</v>
       </c>
-      <c r="C16" s="7">
-        <v>0</v>
-      </c>
-      <c r="D16" s="7">
-        <v>0</v>
-      </c>
-      <c r="E16" s="7">
-        <v>0</v>
-      </c>
-      <c r="F16" s="8" t="s">
+      <c r="C16" s="4">
+        <v>0</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="3">
         <f>B16*D16</f>
         <v>0</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="3">
         <f>B16*E16</f>
         <v>0</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I16" s="3">
         <f>IF(F16="True",70,0)</f>
         <v>0</v>
       </c>
-      <c r="J16" s="6">
+      <c r="J16" s="3">
         <f>B16*C16</f>
         <v>0</v>
       </c>
-      <c r="K16" s="6">
+      <c r="K16" s="3">
         <f>G16+H16+I16+J16+B16</f>
         <v>35000</v>
       </c>
@@ -1157,7 +1169,7 @@
       <c r="K18" s="1"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1165,19 +1177,22 @@
       <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="4">
         <v>0.19</v>
       </c>
-      <c r="D20" s="7">
-        <v>0</v>
-      </c>
-      <c r="E20" s="7">
-        <v>0</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="D20" s="4">
+        <v>0</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1185,39 +1200,48 @@
       <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="3">
         <v>78000</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="4">
         <v>-0.12</v>
       </c>
-      <c r="D21" s="7">
-        <v>0</v>
-      </c>
-      <c r="E21" s="7">
-        <v>0</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="D21" s="4">
+        <v>0</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" t="s">
         <v>36</v>
+      </c>
+      <c r="J21" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="3">
         <v>65000</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="4">
         <v>0.19</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="4">
         <v>-0.05</v>
       </c>
-      <c r="E22" s="7">
-        <v>0</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="E22" s="4">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1225,29 +1249,50 @@
       <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="6">
-        <v>65000</v>
-      </c>
-      <c r="C23" s="7">
+      <c r="B23" s="3">
+        <v>130000</v>
+      </c>
+      <c r="C23" s="4">
         <v>0.19</v>
       </c>
-      <c r="D23" s="7">
-        <v>0</v>
-      </c>
-      <c r="E23" s="7">
+      <c r="D23" s="4">
+        <v>0</v>
+      </c>
+      <c r="E23" s="4">
         <v>-0.06</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="3">
+        <v>23380</v>
+      </c>
+      <c r="C24" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="D24" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="E24" s="6">
+        <v>0</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="A2:A3"/>
@@ -1256,6 +1301,11 @@
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>